<commit_message>
I organized the short stories differently.
</commit_message>
<xml_diff>
--- a/export_scripts/data/pod/SplittingPoD/NewNodeIDs.xlsx
+++ b/export_scripts/data/pod/SplittingPoD/NewNodeIDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinnebancroft/Documents/narratives-final-scripts/export_scripts/data/pod/SplittingPoD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537AA3AA-0389-644E-81C5-E5749777166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C651F2-7294-5349-92A3-6FC9D9486473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17760" yWindow="500" windowWidth="27240" windowHeight="15940" xr2:uid="{84BE45A6-4CD7-DA43-81E8-EC1DC102EC20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{84BE45A6-4CD7-DA43-81E8-EC1DC102EC20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Old ID</t>
   </si>
@@ -84,6 +84,54 @@
   </si>
   <si>
     <t>Tenny McElwayne</t>
+  </si>
+  <si>
+    <t>Evelina Harp</t>
+  </si>
+  <si>
+    <t>Dot Adare</t>
+  </si>
+  <si>
+    <t>Sister Mary Anita Buckendorf</t>
+  </si>
+  <si>
+    <t>Sister Mary Anita</t>
+  </si>
+  <si>
+    <t>Corwin Peace</t>
+  </si>
+  <si>
+    <t>Toddy Crieder</t>
+  </si>
+  <si>
+    <t>Evelina's Former Teachers</t>
+  </si>
+  <si>
+    <t>Dot's Former Teachers</t>
+  </si>
+  <si>
+    <t>Other Children (in school with Evelina)</t>
+  </si>
+  <si>
+    <t>Other Children</t>
+  </si>
+  <si>
+    <t>Other Teachers (at Evelina's school)</t>
+  </si>
+  <si>
+    <t>Other Teachers</t>
+  </si>
+  <si>
+    <t>Clemence Harp</t>
+  </si>
+  <si>
+    <t>Dot's Mother</t>
+  </si>
+  <si>
+    <t>Sister Mary Anita's Father</t>
+  </si>
+  <si>
+    <t>Sister Mary Anita's Family</t>
   </si>
 </sst>
 </file>
@@ -455,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94AF1FC-E5D6-5648-AED9-770554CB07A6}">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,82 +675,130 @@
         <v>414</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>415</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>416</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>417</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>418</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>419</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>421</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>422</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>423</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>424</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>425</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>426</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>427</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>428</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>430</v>
       </c>

</xml_diff>